<commit_message>
fernanda fez a planilha
</commit_message>
<xml_diff>
--- a/doc/ACAP DG PH 8.1 31-03-21.xlsx
+++ b/doc/ACAP DG PH 8.1 31-03-21.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="510" windowWidth="19815" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="390" yWindow="510" windowWidth="19815" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ACAP DG PH 8.1 31-03-21.xls" sheetId="1" r:id="rId1"/>
@@ -514,11 +514,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="119231616"/>
-        <c:axId val="119268096"/>
+        <c:axId val="102007552"/>
+        <c:axId val="102448128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119231616"/>
+        <c:axId val="102007552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -527,7 +527,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119268096"/>
+        <c:crossAx val="102448128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -535,7 +535,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119268096"/>
+        <c:axId val="102448128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -546,7 +546,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119231616"/>
+        <c:crossAx val="102007552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -647,7 +647,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -704,7 +703,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -759,11 +757,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127954944"/>
-        <c:axId val="127956480"/>
+        <c:axId val="63755392"/>
+        <c:axId val="63756928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127954944"/>
+        <c:axId val="63755392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -772,7 +770,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127956480"/>
+        <c:crossAx val="63756928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -780,7 +778,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127956480"/>
+        <c:axId val="63756928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -791,14 +789,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127954944"/>
+        <c:crossAx val="63755392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -892,7 +889,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -949,7 +945,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1004,11 +999,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127988096"/>
-        <c:axId val="127989632"/>
+        <c:axId val="73750016"/>
+        <c:axId val="73751552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127988096"/>
+        <c:axId val="73750016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1017,7 +1012,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127989632"/>
+        <c:crossAx val="73751552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1025,7 +1020,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127989632"/>
+        <c:axId val="73751552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1036,14 +1031,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127988096"/>
+        <c:crossAx val="73750016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1137,7 +1131,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1194,7 +1187,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1249,11 +1241,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127763200"/>
-        <c:axId val="127764736"/>
+        <c:axId val="73783168"/>
+        <c:axId val="73784704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127763200"/>
+        <c:axId val="73783168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1262,7 +1254,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127764736"/>
+        <c:crossAx val="73784704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1270,7 +1262,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127764736"/>
+        <c:axId val="73784704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1281,14 +1273,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127763200"/>
+        <c:crossAx val="73783168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1382,7 +1373,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -1499,11 +1489,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127788160"/>
-        <c:axId val="127789696"/>
+        <c:axId val="73804032"/>
+        <c:axId val="73809920"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127788160"/>
+        <c:axId val="73804032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1512,7 +1502,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127789696"/>
+        <c:crossAx val="73809920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1520,7 +1510,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="127789696"/>
+        <c:axId val="73809920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1531,14 +1521,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127788160"/>
+        <c:crossAx val="73804032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1744,11 +1733,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="120024064"/>
-        <c:axId val="123528704"/>
+        <c:axId val="33138560"/>
+        <c:axId val="33140096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="120024064"/>
+        <c:axId val="33138560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1757,7 +1746,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="123528704"/>
+        <c:crossAx val="33140096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1765,7 +1754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="123528704"/>
+        <c:axId val="33140096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1776,7 +1765,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120024064"/>
+        <c:crossAx val="33138560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1989,11 +1978,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126243200"/>
-        <c:axId val="126245504"/>
+        <c:axId val="33159424"/>
+        <c:axId val="33304576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126243200"/>
+        <c:axId val="33159424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2002,7 +1991,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126245504"/>
+        <c:crossAx val="33304576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2010,7 +1999,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126245504"/>
+        <c:axId val="33304576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2021,7 +2010,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126243200"/>
+        <c:crossAx val="33159424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2122,7 +2111,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2179,7 +2167,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2234,11 +2221,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="128401408"/>
-        <c:axId val="128478592"/>
+        <c:axId val="33335936"/>
+        <c:axId val="33337728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128401408"/>
+        <c:axId val="33335936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2247,7 +2234,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128478592"/>
+        <c:crossAx val="33337728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2255,7 +2242,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128478592"/>
+        <c:axId val="33337728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2266,14 +2253,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128401408"/>
+        <c:crossAx val="33335936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2367,7 +2353,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2424,7 +2409,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2479,11 +2463,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="128198528"/>
-        <c:axId val="128200064"/>
+        <c:axId val="33356800"/>
+        <c:axId val="63574784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="128198528"/>
+        <c:axId val="33356800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2492,7 +2476,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128200064"/>
+        <c:crossAx val="63574784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2500,7 +2484,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="128200064"/>
+        <c:axId val="63574784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2511,14 +2495,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="128198528"/>
+        <c:crossAx val="33356800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2612,7 +2595,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2669,7 +2651,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2724,11 +2705,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126368000"/>
-        <c:axId val="126373888"/>
+        <c:axId val="63585664"/>
+        <c:axId val="63591552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126368000"/>
+        <c:axId val="63585664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2737,7 +2718,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126373888"/>
+        <c:crossAx val="63591552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2745,7 +2726,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126373888"/>
+        <c:axId val="63591552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2756,14 +2737,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126368000"/>
+        <c:crossAx val="63585664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2857,7 +2837,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2914,7 +2893,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -2969,11 +2947,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126401152"/>
-        <c:axId val="126411136"/>
+        <c:axId val="63619072"/>
+        <c:axId val="63620608"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126401152"/>
+        <c:axId val="63619072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2982,7 +2960,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126411136"/>
+        <c:crossAx val="63620608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2990,7 +2968,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126411136"/>
+        <c:axId val="63620608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3001,14 +2979,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126401152"/>
+        <c:crossAx val="63619072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3102,7 +3079,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3159,7 +3135,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3214,11 +3189,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126635008"/>
-        <c:axId val="126640896"/>
+        <c:axId val="63701376"/>
+        <c:axId val="63702912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126635008"/>
+        <c:axId val="63701376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3227,7 +3202,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126640896"/>
+        <c:crossAx val="63702912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3235,7 +3210,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126640896"/>
+        <c:axId val="63702912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3246,14 +3221,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126635008"/>
+        <c:crossAx val="63701376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3347,7 +3321,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3404,7 +3377,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -3459,11 +3431,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="126659968"/>
-        <c:axId val="126665856"/>
+        <c:axId val="63730432"/>
+        <c:axId val="63731968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="126659968"/>
+        <c:axId val="63730432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3472,7 +3444,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126665856"/>
+        <c:crossAx val="63731968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3480,7 +3452,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="126665856"/>
+        <c:axId val="63731968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3491,14 +3463,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="126659968"/>
+        <c:crossAx val="63730432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -12140,8 +12111,8 @@
   </sheetPr>
   <dimension ref="A1:I1249"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12185,7 +12156,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="13"/>
-      <c r="E2" s="4">
+      <c r="I2" s="4">
         <v>1731751</v>
       </c>
     </row>
@@ -12223,11 +12194,11 @@
       </c>
       <c r="F4" s="14">
         <f>AVERAGE(E2:E4)</f>
-        <v>2343460</v>
+        <v>2649314.5</v>
       </c>
       <c r="G4" s="26">
         <f>STDEV(E2:E4)/F4*100</f>
-        <v>23.863287763405179</v>
+        <v>9.5629042890782383</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>21</v>
@@ -12290,7 +12261,7 @@
       </c>
       <c r="H7" s="14">
         <f>F7-$F$4</f>
-        <v>6702171</v>
+        <v>6396316.5</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -12350,7 +12321,7 @@
       </c>
       <c r="H10" s="14">
         <f>F10-$F$4</f>
-        <v>7115436</v>
+        <v>6809581.5</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -12379,7 +12350,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="13"/>
-      <c r="E12" s="5">
+      <c r="I12" s="5">
         <v>5901504</v>
       </c>
     </row>
@@ -12402,15 +12373,15 @@
       </c>
       <c r="F13" s="14">
         <f>AVERAGE(E11:E13)</f>
-        <v>6879406.333333333</v>
+        <v>7368357.5</v>
       </c>
       <c r="G13" s="26">
         <f>STDEV(E11:E13)/F13*100</f>
-        <v>13.167050601950791</v>
+        <v>6.1681421169821071</v>
       </c>
       <c r="H13" s="14">
         <f>F13-$F$4</f>
-        <v>4535946.333333333</v>
+        <v>4719043</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
@@ -12424,7 +12395,7 @@
         <v>0</v>
       </c>
       <c r="D14" s="13"/>
-      <c r="E14" s="5">
+      <c r="I14" s="5">
         <v>10567648</v>
       </c>
     </row>
@@ -12462,15 +12433,15 @@
       </c>
       <c r="F16" s="14">
         <f>AVERAGE(E14:E16)</f>
-        <v>12184201.666666666</v>
+        <v>12992478.5</v>
       </c>
       <c r="G16" s="26">
         <f>STDEV(E14:E16)/F16*100</f>
-        <v>12.283975865603097</v>
+        <v>5.7616794044659709</v>
       </c>
       <c r="H16" s="14">
         <f>F16-$F$4</f>
-        <v>9840741.666666666</v>
+        <v>10343164</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -12530,7 +12501,7 @@
       </c>
       <c r="H19" s="14">
         <f>F19-$F$4</f>
-        <v>10234214</v>
+        <v>9928359.5</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -12590,7 +12561,7 @@
       </c>
       <c r="H22" s="14">
         <f>F22-$F$4</f>
-        <v>5273997</v>
+        <v>4968142.5</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -12650,7 +12621,7 @@
       </c>
       <c r="H25" s="14">
         <f>F25-$F$4</f>
-        <v>6020715.666666667</v>
+        <v>5714861.166666667</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -12710,7 +12681,7 @@
       </c>
       <c r="H28" s="14">
         <f>F28-$F$4</f>
-        <v>4632807.666666667</v>
+        <v>4326953.166666667</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -12770,7 +12741,7 @@
       </c>
       <c r="H31" s="14">
         <f>F31-$F$4</f>
-        <v>6220279.333333334</v>
+        <v>5914424.833333334</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -12830,7 +12801,7 @@
       </c>
       <c r="H34" s="14">
         <f>F34-$F$4</f>
-        <v>3416324.666666667</v>
+        <v>3110470.166666667</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -12890,7 +12861,7 @@
       </c>
       <c r="H37" s="14">
         <f>F37-$F$4</f>
-        <v>8161659.333333334</v>
+        <v>7855804.833333334</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -12950,7 +12921,7 @@
       </c>
       <c r="H40" s="14">
         <f>F40-$F$4</f>
-        <v>9644986</v>
+        <v>9339131.5</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -13010,7 +12981,7 @@
       </c>
       <c r="H43" s="14">
         <f>F43-$F$4</f>
-        <v>14347909.333333334</v>
+        <v>14042054.833333334</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -13070,7 +13041,7 @@
       </c>
       <c r="H46" s="14">
         <f>F46-$F$4</f>
-        <v>3459713.666666667</v>
+        <v>3153859.166666667</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -13130,7 +13101,7 @@
       </c>
       <c r="H49" s="14">
         <f>F49-$F$4</f>
-        <v>5670352.333333333</v>
+        <v>5364497.833333333</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -13432,7 +13403,7 @@
         <v>10943466</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="16" t="s">
         <v>37</v>
       </c>
@@ -13447,7 +13418,7 @@
         <v>15977062</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="16" t="s">
         <v>37</v>
       </c>
@@ -13462,7 +13433,7 @@
         <v>14704173</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="16" t="s">
         <v>37</v>
       </c>
@@ -13492,7 +13463,7 @@
         <v>10776458.333333334</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="16" t="s">
         <v>37</v>
       </c>
@@ -13507,7 +13478,7 @@
         <v>8288290</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="16" t="s">
         <v>37</v>
       </c>
@@ -13522,7 +13493,7 @@
         <v>7265297</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="16" t="s">
         <v>37</v>
       </c>
@@ -13552,7 +13523,7 @@
         <v>3645340.0000000005</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="16" t="s">
         <v>37</v>
       </c>
@@ -13563,11 +13534,11 @@
         <v>0</v>
       </c>
       <c r="D71" s="13"/>
-      <c r="E71" s="6">
+      <c r="I71" s="6">
         <v>13231302</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="16" t="s">
         <v>37</v>
       </c>
@@ -13582,7 +13553,7 @@
         <v>9709998</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="16" t="s">
         <v>37</v>
       </c>
@@ -13601,18 +13572,18 @@
       </c>
       <c r="F73" s="14">
         <f>AVERAGE(E71:E73)</f>
-        <v>11315510.666666666</v>
+        <v>10357615</v>
       </c>
       <c r="G73" s="26">
         <f>STDEV(E71:E73)/F73*100</f>
-        <v>15.739802683872933</v>
+        <v>8.8424675431880466</v>
       </c>
       <c r="H73" s="14">
         <f>F73-$F$52</f>
-        <v>7198660</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+        <v>6240764.333333334</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="16" t="s">
         <v>37</v>
       </c>
@@ -13623,11 +13594,8 @@
         <v>0</v>
       </c>
       <c r="D74" s="13"/>
-      <c r="E74" s="6">
-        <v>10576828</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="16" t="s">
         <v>37</v>
       </c>
@@ -13641,8 +13609,11 @@
       <c r="E75" s="6">
         <v>7555431</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="I75" s="6">
+        <v>10576828</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="16" t="s">
         <v>37</v>
       </c>
@@ -13661,18 +13632,18 @@
       </c>
       <c r="F76" s="14">
         <f>AVERAGE(E74:E76)</f>
-        <v>8692026.666666666</v>
+        <v>7749626</v>
       </c>
       <c r="G76" s="26">
         <f>STDEV(E74:E76)/F76*100</f>
-        <v>18.911550952096569</v>
+        <v>3.5438252471157088</v>
       </c>
       <c r="H76" s="14">
         <f>F76-$F$52</f>
-        <v>4575176</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+        <v>3632775.3333333335</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="16" t="s">
         <v>37</v>
       </c>
@@ -13683,11 +13654,11 @@
         <v>0</v>
       </c>
       <c r="D77" s="13"/>
-      <c r="E77" s="6">
+      <c r="I77" s="6">
         <v>12869044</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="16" t="s">
         <v>37</v>
       </c>
@@ -13702,7 +13673,7 @@
         <v>8935418</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="16" t="s">
         <v>37</v>
       </c>
@@ -13721,18 +13692,18 @@
       </c>
       <c r="F79" s="14">
         <f>AVERAGE(E77:E79)</f>
-        <v>10548118.666666666</v>
+        <v>9387656</v>
       </c>
       <c r="G79" s="26">
         <f>STDEV(E77:E79)/F79*100</f>
-        <v>19.531711866726724</v>
+        <v>6.812788123259776</v>
       </c>
       <c r="H79" s="14">
         <f>F79-$F$52</f>
-        <v>6431268</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+        <v>5270805.333333334</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="16" t="s">
         <v>37</v>
       </c>
@@ -13747,7 +13718,7 @@
         <v>6453973</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="16" t="s">
         <v>37</v>
       </c>
@@ -13762,7 +13733,7 @@
         <v>5840544</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="16" t="s">
         <v>37</v>
       </c>
@@ -13792,7 +13763,7 @@
         <v>2201616.0000000005</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="16" t="s">
         <v>37</v>
       </c>
@@ -13807,7 +13778,7 @@
         <v>13639838</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="16" t="s">
         <v>37</v>
       </c>
@@ -13822,7 +13793,7 @@
         <v>12768917</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="16" t="s">
         <v>37</v>
       </c>
@@ -13852,7 +13823,7 @@
         <v>9407892.333333334</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="16" t="s">
         <v>37</v>
       </c>
@@ -13867,7 +13838,7 @@
         <v>12300462</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="16" t="s">
         <v>37</v>
       </c>
@@ -13878,11 +13849,11 @@
         <v>0</v>
       </c>
       <c r="D87" s="13"/>
-      <c r="E87" s="7">
+      <c r="I87" s="7">
         <v>14835699</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="16" t="s">
         <v>37</v>
       </c>
@@ -13901,18 +13872,18 @@
       </c>
       <c r="F88" s="14">
         <f>AVERAGE(E86:E88)</f>
-        <v>13070376.333333334</v>
+        <v>12187715</v>
       </c>
       <c r="G88" s="26">
         <f>STDEV(E86:E88)/F88*100</f>
-        <v>11.728553422353972</v>
+        <v>1.3082709639737995</v>
       </c>
       <c r="H88" s="14">
         <f>F88-$F$52</f>
-        <v>8953525.6666666679</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+        <v>8070864.333333334</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="16" t="s">
         <v>37</v>
       </c>
@@ -13927,7 +13898,7 @@
         <v>16608458</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="16" t="s">
         <v>37</v>
       </c>
@@ -13942,7 +13913,7 @@
         <v>16798036</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="16" t="s">
         <v>37</v>
       </c>
@@ -13956,23 +13927,23 @@
         <f>CONCATENATE(A91,B91,C91)</f>
         <v>Com ABAP10BP3_30</v>
       </c>
-      <c r="E91" s="7">
-        <v>20880562</v>
-      </c>
       <c r="F91" s="14">
         <f>AVERAGE(E89:E91)</f>
-        <v>18095685.333333332</v>
+        <v>16703247</v>
       </c>
       <c r="G91" s="26">
         <f>STDEV(E89:E91)/F91*100</f>
-        <v>13.33818478736816</v>
+        <v>0.80254988364707358</v>
       </c>
       <c r="H91" s="14">
         <f>F91-$F$52</f>
-        <v>13978834.666666666</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+        <v>12586396.333333334</v>
+      </c>
+      <c r="I91" s="7">
+        <v>20880562</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="16" t="s">
         <v>37</v>
       </c>
@@ -13987,7 +13958,7 @@
         <v>6838625</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="16" t="s">
         <v>37</v>
       </c>
@@ -14002,7 +13973,7 @@
         <v>6971561</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="16" t="s">
         <v>37</v>
       </c>
@@ -14032,7 +14003,7 @@
         <v>2820908.3333333335</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="16" t="s">
         <v>37</v>
       </c>
@@ -14047,7 +14018,7 @@
         <v>8317005</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="16" t="s">
         <v>37</v>
       </c>
@@ -14062,7 +14033,7 @@
         <v>8154386</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="16" t="s">
         <v>37</v>
       </c>
@@ -14092,7 +14063,7 @@
         <v>4615890.333333334</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="12" t="s">
         <v>19</v>
       </c>
@@ -14103,11 +14074,11 @@
         <v>5</v>
       </c>
       <c r="D98" s="13"/>
-      <c r="E98" s="4">
+      <c r="I98" s="4">
         <v>1783372</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="12" t="s">
         <v>19</v>
       </c>
@@ -14122,7 +14093,7 @@
         <v>2875034</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="12" t="s">
         <v>19</v>
       </c>
@@ -14141,17 +14112,17 @@
       </c>
       <c r="F100" s="14">
         <f>AVERAGE(E98:E100)</f>
-        <v>2382297.3333333335</v>
+        <v>2681760</v>
       </c>
       <c r="G100" s="26">
         <f>STDEV(E98:E100)/F100*100</f>
-        <v>23.234871199040366</v>
+        <v>10.192213772078693</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="12" t="s">
         <v>19</v>
       </c>
@@ -14166,7 +14137,7 @@
         <v>30359206</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="12" t="s">
         <v>19</v>
       </c>
@@ -14181,7 +14152,7 @@
         <v>35959968</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="12" t="s">
         <v>19</v>
       </c>
@@ -14208,10 +14179,10 @@
       </c>
       <c r="H103" s="14">
         <f>F103-$F$100</f>
-        <v>31723668.666666668</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+        <v>31424206</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="12" t="s">
         <v>19</v>
       </c>
@@ -14226,7 +14197,7 @@
         <v>39059124</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="12" t="s">
         <v>19</v>
       </c>
@@ -14241,7 +14212,7 @@
         <v>35503096</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="12" t="s">
         <v>19</v>
       </c>
@@ -14255,23 +14226,23 @@
         <f>CONCATENATE(A106,B106,C106)</f>
         <v>Sem ABAPC25</v>
       </c>
-      <c r="E106" s="5">
-        <v>45666972</v>
-      </c>
       <c r="F106" s="14">
         <f>AVERAGE(E104:E106)</f>
-        <v>40076397.333333336</v>
+        <v>37281110</v>
       </c>
       <c r="G106" s="26">
         <f>STDEV(E104:E106)/F106*100</f>
-        <v>12.869756464333273</v>
+        <v>6.7446798469499329</v>
       </c>
       <c r="H106" s="14">
         <f>F106-$F$100</f>
-        <v>37694100</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+        <v>34599350</v>
+      </c>
+      <c r="I106" s="5">
+        <v>45666972</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="12" t="s">
         <v>19</v>
       </c>
@@ -14286,7 +14257,7 @@
         <v>27264198</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="12" t="s">
         <v>19</v>
       </c>
@@ -14297,11 +14268,11 @@
         <v>5</v>
       </c>
       <c r="D108" s="13"/>
-      <c r="E108" s="5">
+      <c r="I108" s="5">
         <v>21339448</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="12" t="s">
         <v>19</v>
       </c>
@@ -14320,18 +14291,18 @@
       </c>
       <c r="F109" s="14">
         <f>AVERAGE(E107:E109)</f>
-        <v>26518585.333333332</v>
+        <v>29108154</v>
       </c>
       <c r="G109" s="26">
         <f>STDEV(E107:E109)/F109*100</f>
-        <v>18.287221685146658</v>
+        <v>8.9588215852480477</v>
       </c>
       <c r="H109" s="14">
         <f>F109-$F$100</f>
-        <v>24136288</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+        <v>26426394</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="12" t="s">
         <v>19</v>
       </c>
@@ -14342,11 +14313,11 @@
         <v>5</v>
       </c>
       <c r="D110" s="13"/>
-      <c r="E110" s="5">
+      <c r="I110" s="5">
         <v>42401340</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="12" t="s">
         <v>19</v>
       </c>
@@ -14361,7 +14332,7 @@
         <v>48952736</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="12" t="s">
         <v>19</v>
       </c>
@@ -14380,15 +14351,15 @@
       </c>
       <c r="F112" s="14">
         <f>AVERAGE(E110:E112)</f>
-        <v>48268802.666666664</v>
+        <v>51202534</v>
       </c>
       <c r="G112" s="26">
         <f>STDEV(E110:E112)/F112*100</f>
-        <v>11.512925347337548</v>
+        <v>6.2139402010843146</v>
       </c>
       <c r="H112" s="14">
         <f>F112-$F$100</f>
-        <v>45886505.333333328</v>
+        <v>48520774</v>
       </c>
     </row>
     <row r="113" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -14448,7 +14419,7 @@
       </c>
       <c r="H115" s="14">
         <f>F115-$F$100</f>
-        <v>44959550.666666664</v>
+        <v>44660088</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -14508,7 +14479,7 @@
       </c>
       <c r="H118" s="14">
         <f>F118-$F$100</f>
-        <v>27708229.333333336</v>
+        <v>27408766.666666668</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -14568,7 +14539,7 @@
       </c>
       <c r="H121" s="14">
         <f>F121-$F$100</f>
-        <v>30857002</v>
+        <v>30557539.333333332</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -14628,7 +14599,7 @@
       </c>
       <c r="H124" s="14">
         <f>F124-$F$100</f>
-        <v>24724303.333333336</v>
+        <v>24424840.666666668</v>
       </c>
     </row>
     <row r="125" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -14688,7 +14659,7 @@
       </c>
       <c r="H127" s="14">
         <f>F127-$F$100</f>
-        <v>29647090</v>
+        <v>29347627.333333332</v>
       </c>
     </row>
     <row r="128" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -14748,7 +14719,7 @@
       </c>
       <c r="H130" s="14">
         <f>F130-$F$100</f>
-        <v>16295288.666666666</v>
+        <v>15995826</v>
       </c>
     </row>
     <row r="131" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -14808,7 +14779,7 @@
       </c>
       <c r="H133" s="14">
         <f>F133-$F$100</f>
-        <v>39448480</v>
+        <v>39149017.333333336</v>
       </c>
     </row>
     <row r="134" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -14868,7 +14839,7 @@
       </c>
       <c r="H136" s="14">
         <f>F136-$F$100</f>
-        <v>40529361.333333328</v>
+        <v>40229898.666666664</v>
       </c>
     </row>
     <row r="137" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -14928,7 +14899,7 @@
       </c>
       <c r="H139" s="14">
         <f>F139-$F$100</f>
-        <v>56173876</v>
+        <v>55874413.333333336</v>
       </c>
     </row>
     <row r="140" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -14988,7 +14959,7 @@
       </c>
       <c r="H142" s="14">
         <f>F142-$F$100</f>
-        <v>17431792</v>
+        <v>17132329.333333332</v>
       </c>
     </row>
     <row r="143" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -15048,7 +15019,7 @@
       </c>
       <c r="H145" s="14">
         <f>F145-$F$100</f>
-        <v>28917476.666666668</v>
+        <v>28618014</v>
       </c>
     </row>
     <row r="146" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
@@ -63365,7 +63336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K151"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -63587,7 +63558,7 @@
       </c>
       <c r="C13">
         <f>VLOOKUP(CONCATENATE($C$1,A13,B13),'Dados planilhados'!D:F,3,FALSE)</f>
-        <v>40076397.333333336</v>
+        <v>37281110</v>
       </c>
       <c r="D13">
         <f>VLOOKUP(CONCATENATE($D$1,A13,B13),'Dados planilhados'!D:F,3,FALSE)</f>
@@ -63731,7 +63702,7 @@
       </c>
       <c r="C22">
         <f>VLOOKUP(CONCATENATE($C$1,A22,B22),'Dados planilhados'!D:F,3,FALSE)</f>
-        <v>6879406.333333333</v>
+        <v>7368357.5</v>
       </c>
       <c r="D22">
         <f>VLOOKUP(CONCATENATE($D$1,A22,B22),'Dados planilhados'!D:F,3,FALSE)</f>
@@ -63747,7 +63718,7 @@
       </c>
       <c r="C23">
         <f>VLOOKUP(CONCATENATE($C$1,A23,B23),'Dados planilhados'!D:F,3,FALSE)</f>
-        <v>26518585.333333332</v>
+        <v>29108154</v>
       </c>
       <c r="D23">
         <f>VLOOKUP(CONCATENATE($D$1,A23,B23),'Dados planilhados'!D:F,3,FALSE)</f>
@@ -63891,7 +63862,7 @@
       </c>
       <c r="C32">
         <f>VLOOKUP(CONCATENATE($C$1,A32,B32),'Dados planilhados'!D:F,3,FALSE)</f>
-        <v>12184201.666666666</v>
+        <v>12992478.5</v>
       </c>
       <c r="D32">
         <f>VLOOKUP(CONCATENATE($D$1,A32,B32),'Dados planilhados'!D:F,3,FALSE)</f>
@@ -63907,7 +63878,7 @@
       </c>
       <c r="C33">
         <f>VLOOKUP(CONCATENATE($C$1,A33,B33),'Dados planilhados'!D:F,3,FALSE)</f>
-        <v>48268802.666666664</v>
+        <v>51202534</v>
       </c>
       <c r="D33">
         <f>VLOOKUP(CONCATENATE($D$1,A33,B33),'Dados planilhados'!D:F,3,FALSE)</f>
@@ -64375,7 +64346,7 @@
       </c>
       <c r="D62">
         <f>VLOOKUP(CONCATENATE($D$1,A62,B62),'Dados planilhados'!D:F,3,FALSE)</f>
-        <v>11315510.666666666</v>
+        <v>10357615</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -64535,7 +64506,7 @@
       </c>
       <c r="D72">
         <f>VLOOKUP(CONCATENATE($D$1,A72,B72),'Dados planilhados'!D:F,3,FALSE)</f>
-        <v>8692026.666666666</v>
+        <v>7749626</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -64695,7 +64666,7 @@
       </c>
       <c r="D82">
         <f>VLOOKUP(CONCATENATE($D$1,A82,B82),'Dados planilhados'!D:F,3,FALSE)</f>
-        <v>10548118.666666666</v>
+        <v>9387656</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -65175,7 +65146,7 @@
       </c>
       <c r="D112">
         <f>VLOOKUP(CONCATENATE($D$1,A112,B112),'Dados planilhados'!D:F,3,FALSE)</f>
-        <v>13070376.333333334</v>
+        <v>12187715</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -65335,7 +65306,7 @@
       </c>
       <c r="D122">
         <f>VLOOKUP(CONCATENATE($D$1,A122,B122),'Dados planilhados'!D:F,3,FALSE)</f>
-        <v>18095685.333333332</v>
+        <v>16703247</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>